<commit_message>
got my models up thanks to tb_liu
</commit_message>
<xml_diff>
--- a/data/performance_sheets/BA47 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets/BA47 Overall Model Peformance Results.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="805" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR1 - DN1 (70-30)" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR1 - DN2 (70-30)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR2 - DN1 (70-30)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR2 - DN2 (70-30)" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - NLR1 - DN1 (70-30)" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - NLR1 - DN2 (70-30)" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - NLR2 - DN1 (70-30)" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - NLR2 - DN2 (70-30)" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Option 1 - LR1 - DN1 (70-30)" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Option 1 - LR1 - DN2 (70-30)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Option 1 - LR2 - DN1 (70-30)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Option 1 - LR2 - DN2 (70-30)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Option 1 - NLR1 - DN1 (70-30)" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Option 1 - NLR1 - DN2 (70-30)" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Option 1 - NLR2 - DN1 (70-30)" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Option 1 - NLR2 - DN2 (70-30)" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191028" fullCalcOnLoad="1"/>
@@ -626,7 +626,7 @@
     <row r="4" ht="30" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  </t>
+          <t>  </t>
         </is>
       </c>
     </row>
@@ -862,25 +862,61 @@
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="B10" s="5" t="n"/>
-      <c r="C10" s="5" t="n"/>
-      <c r="D10" s="5" t="n"/>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="5" t="n"/>
-      <c r="G10" s="5" t="n"/>
-      <c r="H10" s="5" t="n"/>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>{'weights': 'distance', 'n_neighbors': 7}</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>0.06169247645418674</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.1755197917099006</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>2.047117853751199</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0.2483797021783115</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>35.91403333838602</v>
+      </c>
       <c r="I10" s="10" t="inlineStr">
         <is>
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="J10" s="9" t="n"/>
-      <c r="K10" s="9" t="n"/>
-      <c r="L10" s="9" t="n"/>
-      <c r="M10" s="9" t="n"/>
-      <c r="N10" s="9" t="n"/>
-      <c r="O10" s="9" t="n"/>
-      <c r="P10" s="9" t="n"/>
+      <c r="J10" s="9" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K10" s="9" t="inlineStr">
+        <is>
+          <t>{'weights': 'uniform', 'n_neighbors': 9}</t>
+        </is>
+      </c>
+      <c r="L10" s="9" t="n">
+        <v>0.07228434603797196</v>
+      </c>
+      <c r="M10" s="9" t="n">
+        <v>0.1879488257881691</v>
+      </c>
+      <c r="N10" s="9" t="n">
+        <v>2.090141726951515</v>
+      </c>
+      <c r="O10" s="9" t="n">
+        <v>0.268857482763586</v>
+      </c>
+      <c r="P10" s="9" t="n">
+        <v>37.55858763901023</v>
+      </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
@@ -1162,25 +1198,61 @@
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="B18" s="5" t="n"/>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 60, 'max_samples': 0.6, 'max_features': 0.5}</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>0.06106197294961744</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.1740955239098886</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>2.192313225776449</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>0.2471072094246087</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>35.54666383416053</v>
+      </c>
       <c r="I18" s="10" t="inlineStr">
         <is>
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="J18" s="9" t="n"/>
-      <c r="K18" s="9" t="n"/>
-      <c r="L18" s="9" t="n"/>
-      <c r="M18" s="9" t="n"/>
-      <c r="N18" s="9" t="n"/>
-      <c r="O18" s="9" t="n"/>
-      <c r="P18" s="9" t="n"/>
+      <c r="J18" s="9" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K18" s="9" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 190, 'max_samples': 0.5, 'max_features': 0.6}</t>
+        </is>
+      </c>
+      <c r="L18" s="9" t="n">
+        <v>0.06255948100867433</v>
+      </c>
+      <c r="M18" s="9" t="n">
+        <v>0.1746550172303896</v>
+      </c>
+      <c r="N18" s="9" t="n">
+        <v>2.147709003343623</v>
+      </c>
+      <c r="O18" s="9" t="n">
+        <v>0.2501189337268859</v>
+      </c>
+      <c r="P18" s="9" t="n">
+        <v>35.63859024486854</v>
+      </c>
     </row>
     <row r="19" ht="121.5" customHeight="1">
       <c r="A19" s="6" t="inlineStr">
@@ -1495,7 +1567,7 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  </t>
+          <t>  </t>
         </is>
       </c>
     </row>
@@ -1731,25 +1803,61 @@
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="B11" s="5" t="n"/>
-      <c r="C11" s="5" t="n"/>
-      <c r="D11" s="5" t="n"/>
-      <c r="E11" s="5" t="n"/>
-      <c r="F11" s="5" t="n"/>
-      <c r="G11" s="5" t="n"/>
-      <c r="H11" s="5" t="n"/>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>{'weights': 'uniform', 'n_neighbors': 9}</t>
+        </is>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>0.902979907324597</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>0.726788484137497</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>0.4970110362517109</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>0.9502525492334114</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <v>36.71832616693433</v>
+      </c>
       <c r="I11" s="10" t="inlineStr">
         <is>
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="J11" s="9" t="n"/>
-      <c r="K11" s="9" t="n"/>
-      <c r="L11" s="9" t="n"/>
-      <c r="M11" s="9" t="n"/>
-      <c r="N11" s="9" t="n"/>
-      <c r="O11" s="9" t="n"/>
-      <c r="P11" s="9" t="n"/>
+      <c r="J11" s="9" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K11" s="9" t="inlineStr">
+        <is>
+          <t>{'weights': 'uniform', 'n_neighbors': 9}</t>
+        </is>
+      </c>
+      <c r="L11" s="9" t="n">
+        <v>0.9089306685964818</v>
+      </c>
+      <c r="M11" s="9" t="n">
+        <v>0.7474075270914161</v>
+      </c>
+      <c r="N11" s="9" t="n">
+        <v>0.505646992268636</v>
+      </c>
+      <c r="O11" s="9" t="n">
+        <v>0.9533785547181569</v>
+      </c>
+      <c r="P11" s="9" t="n">
+        <v>37.67978511518434</v>
+      </c>
     </row>
     <row r="12" ht="30.75" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
@@ -2031,25 +2139,61 @@
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="B19" s="5" t="n"/>
-      <c r="C19" s="5" t="n"/>
-      <c r="D19" s="5" t="n"/>
-      <c r="E19" s="5" t="n"/>
-      <c r="F19" s="5" t="n"/>
-      <c r="G19" s="5" t="n"/>
-      <c r="H19" s="5" t="n"/>
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>0.81775343298557</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>0.5415527268918022</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <v>0.4689246517851805</v>
+      </c>
+      <c r="G19" s="5" t="n">
+        <v>0.9042972039023288</v>
+      </c>
+      <c r="H19" s="5" t="n">
+        <v>27.02378782370029</v>
+      </c>
       <c r="I19" s="10" t="inlineStr">
         <is>
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="J19" s="9" t="n"/>
-      <c r="K19" s="9" t="n"/>
-      <c r="L19" s="9" t="n"/>
-      <c r="M19" s="9" t="n"/>
-      <c r="N19" s="9" t="n"/>
-      <c r="O19" s="9" t="n"/>
-      <c r="P19" s="9" t="n"/>
+      <c r="J19" s="9" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K19" s="9" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
+        </is>
+      </c>
+      <c r="L19" s="9" t="n">
+        <v>0.7946782105022721</v>
+      </c>
+      <c r="M19" s="9" t="n">
+        <v>0.5651145284831797</v>
+      </c>
+      <c r="N19" s="9" t="n">
+        <v>0.4646199786191351</v>
+      </c>
+      <c r="O19" s="9" t="n">
+        <v>0.891447256152753</v>
+      </c>
+      <c r="P19" s="9" t="n">
+        <v>28.33659304107054</v>
+      </c>
     </row>
     <row r="20" ht="60.75" customHeight="1">
       <c r="A20" s="6" t="inlineStr">
@@ -2593,25 +2737,61 @@
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="B10" s="5" t="n"/>
-      <c r="C10" s="5" t="n"/>
-      <c r="D10" s="5" t="n"/>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="5" t="n"/>
-      <c r="G10" s="5" t="n"/>
-      <c r="H10" s="5" t="n"/>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>{'weights': 'distance', 'n_neighbors': 3}</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>56.6033509163731</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>5.556175346219287</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>2.079088248344954</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>7.523519848872142</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>46.7100680616327</v>
+      </c>
       <c r="I10" s="10" t="inlineStr">
         <is>
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="J10" s="9" t="n"/>
-      <c r="K10" s="9" t="n"/>
-      <c r="L10" s="9" t="n"/>
-      <c r="M10" s="9" t="n"/>
-      <c r="N10" s="9" t="n"/>
-      <c r="O10" s="9" t="n"/>
-      <c r="P10" s="9" t="n"/>
+      <c r="J10" s="9" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K10" s="9" t="inlineStr">
+        <is>
+          <t>{'weights': 'uniform', 'n_neighbors': 2}</t>
+        </is>
+      </c>
+      <c r="L10" s="9" t="n">
+        <v>74.42855695995218</v>
+      </c>
+      <c r="M10" s="9" t="n">
+        <v>6.410130238374999</v>
+      </c>
+      <c r="N10" s="9" t="n">
+        <v>2.489330944246513</v>
+      </c>
+      <c r="O10" s="9" t="n">
+        <v>8.627198673958551</v>
+      </c>
+      <c r="P10" s="9" t="n">
+        <v>54.89750309952216</v>
+      </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
@@ -2893,25 +3073,61 @@
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="B18" s="5" t="n"/>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>40.13351091669136</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>4.990873150410834</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>1.889927608119</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>6.335101492217103</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>42.67485897217583</v>
+      </c>
       <c r="I18" s="10" t="inlineStr">
         <is>
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="J18" s="9" t="n"/>
-      <c r="K18" s="9" t="n"/>
-      <c r="L18" s="9" t="n"/>
-      <c r="M18" s="9" t="n"/>
-      <c r="N18" s="9" t="n"/>
-      <c r="O18" s="9" t="n"/>
-      <c r="P18" s="9" t="n"/>
+      <c r="J18" s="9" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K18" s="9" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
+        </is>
+      </c>
+      <c r="L18" s="9" t="n">
+        <v>40.8701185757654</v>
+      </c>
+      <c r="M18" s="9" t="n">
+        <v>5.115923879240666</v>
+      </c>
+      <c r="N18" s="9" t="n">
+        <v>1.876979339387862</v>
+      </c>
+      <c r="O18" s="9" t="n">
+        <v>6.392974157289031</v>
+      </c>
+      <c r="P18" s="9" t="n">
+        <v>43.77639122910413</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
@@ -3455,25 +3671,61 @@
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="B10" s="5" t="n"/>
-      <c r="C10" s="5" t="n"/>
-      <c r="D10" s="5" t="n"/>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="5" t="n"/>
-      <c r="G10" s="5" t="n"/>
-      <c r="H10" s="5" t="n"/>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>{'weights': 'distance', 'n_neighbors': 2}</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>50.94849455514187</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>5.561231169862104</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>1.537955702959697</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>7.137821415189783</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>46.45187852594111</v>
+      </c>
       <c r="I10" s="10" t="inlineStr">
         <is>
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="J10" s="9" t="n"/>
-      <c r="K10" s="9" t="n"/>
-      <c r="L10" s="9" t="n"/>
-      <c r="M10" s="9" t="n"/>
-      <c r="N10" s="9" t="n"/>
-      <c r="O10" s="9" t="n"/>
-      <c r="P10" s="9" t="n"/>
+      <c r="J10" s="9" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K10" s="9" t="inlineStr">
+        <is>
+          <t>{'weights': 'distance', 'n_neighbors': 3}</t>
+        </is>
+      </c>
+      <c r="L10" s="9" t="n">
+        <v>37.17930816961194</v>
+      </c>
+      <c r="M10" s="9" t="n">
+        <v>4.410696307769305</v>
+      </c>
+      <c r="N10" s="9" t="n">
+        <v>1.82274778877643</v>
+      </c>
+      <c r="O10" s="9" t="n">
+        <v>6.097483757224118</v>
+      </c>
+      <c r="P10" s="9" t="n">
+        <v>38.14012003423365</v>
+      </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
@@ -3755,25 +4007,61 @@
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="B18" s="5" t="n"/>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>41.41475998952957</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>5.234000340789668</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>1.856077845819582</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>6.435430054746114</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>44.90751161968928</v>
+      </c>
       <c r="I18" s="10" t="inlineStr">
         <is>
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="J18" s="9" t="n"/>
-      <c r="K18" s="9" t="n"/>
-      <c r="L18" s="9" t="n"/>
-      <c r="M18" s="9" t="n"/>
-      <c r="N18" s="9" t="n"/>
-      <c r="O18" s="9" t="n"/>
-      <c r="P18" s="9" t="n"/>
+      <c r="J18" s="9" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K18" s="9" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
+        </is>
+      </c>
+      <c r="L18" s="9" t="n">
+        <v>37.20632708055398</v>
+      </c>
+      <c r="M18" s="9" t="n">
+        <v>4.893792872582334</v>
+      </c>
+      <c r="N18" s="9" t="n">
+        <v>1.765480532374836</v>
+      </c>
+      <c r="O18" s="9" t="n">
+        <v>6.099698933599426</v>
+      </c>
+      <c r="P18" s="9" t="n">
+        <v>42.3714961027795</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
@@ -4297,25 +4585,61 @@
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="B10" s="5" t="n"/>
-      <c r="C10" s="5" t="n"/>
-      <c r="D10" s="5" t="n"/>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="5" t="n"/>
-      <c r="G10" s="5" t="n"/>
-      <c r="H10" s="5" t="n"/>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>{'weights': 'uniform', 'n_neighbors': 9}</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>0.06235240775096344</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.1817857397937433</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>21207547243030.75</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0.2497046410280823</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>37.57252129791878</v>
+      </c>
       <c r="I10" s="10" t="inlineStr">
         <is>
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="J10" s="9" t="n"/>
-      <c r="K10" s="9" t="n"/>
-      <c r="L10" s="9" t="n"/>
-      <c r="M10" s="9" t="n"/>
-      <c r="N10" s="9" t="n"/>
-      <c r="O10" s="9" t="n"/>
-      <c r="P10" s="9" t="n"/>
+      <c r="J10" s="9" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K10" s="9" t="inlineStr">
+        <is>
+          <t>{'weights': 'uniform', 'n_neighbors': 9}</t>
+        </is>
+      </c>
+      <c r="L10" s="9" t="n">
+        <v>0.06235240775096344</v>
+      </c>
+      <c r="M10" s="9" t="n">
+        <v>0.1817857397937433</v>
+      </c>
+      <c r="N10" s="9" t="n">
+        <v>21207547243030.75</v>
+      </c>
+      <c r="O10" s="9" t="n">
+        <v>0.2497046410280823</v>
+      </c>
+      <c r="P10" s="9" t="n">
+        <v>37.57252129791878</v>
+      </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
@@ -4597,25 +4921,61 @@
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="B18" s="5" t="n"/>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>0.06326782872181687</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.1849570189069101</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>25930799268791.21</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>0.2515309697071453</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>38.01894093918599</v>
+      </c>
       <c r="I18" s="10" t="inlineStr">
         <is>
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="J18" s="9" t="n"/>
-      <c r="K18" s="9" t="n"/>
-      <c r="L18" s="9" t="n"/>
-      <c r="M18" s="9" t="n"/>
-      <c r="N18" s="9" t="n"/>
-      <c r="O18" s="9" t="n"/>
-      <c r="P18" s="9" t="n"/>
+      <c r="J18" s="9" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K18" s="9" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
+        </is>
+      </c>
+      <c r="L18" s="9" t="n">
+        <v>0.06326782872181687</v>
+      </c>
+      <c r="M18" s="9" t="n">
+        <v>0.1849570189069101</v>
+      </c>
+      <c r="N18" s="9" t="n">
+        <v>25930799268791.21</v>
+      </c>
+      <c r="O18" s="9" t="n">
+        <v>0.2515309697071453</v>
+      </c>
+      <c r="P18" s="9" t="n">
+        <v>38.01894093918599</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
@@ -5139,25 +5499,61 @@
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="B10" s="5" t="n"/>
-      <c r="C10" s="5" t="n"/>
-      <c r="D10" s="5" t="n"/>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="5" t="n"/>
-      <c r="G10" s="5" t="n"/>
-      <c r="H10" s="5" t="n"/>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>{'weights': 'uniform', 'n_neighbors': 9}</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>1.05365327372825</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.5595554917670698</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0.592187535448938</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>1.026476143769669</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>26.35914467881757</v>
+      </c>
       <c r="I10" s="10" t="inlineStr">
         <is>
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="J10" s="9" t="n"/>
-      <c r="K10" s="9" t="n"/>
-      <c r="L10" s="9" t="n"/>
-      <c r="M10" s="9" t="n"/>
-      <c r="N10" s="9" t="n"/>
-      <c r="O10" s="9" t="n"/>
-      <c r="P10" s="9" t="n"/>
+      <c r="J10" s="9" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K10" s="9" t="inlineStr">
+        <is>
+          <t>{'weights': 'uniform', 'n_neighbors': 9}</t>
+        </is>
+      </c>
+      <c r="L10" s="9" t="n">
+        <v>1.05365327372825</v>
+      </c>
+      <c r="M10" s="9" t="n">
+        <v>0.5595554917670698</v>
+      </c>
+      <c r="N10" s="9" t="n">
+        <v>0.592187535448938</v>
+      </c>
+      <c r="O10" s="9" t="n">
+        <v>1.026476143769669</v>
+      </c>
+      <c r="P10" s="9" t="n">
+        <v>26.35914467881757</v>
+      </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
@@ -5439,25 +5835,61 @@
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="B18" s="5" t="n"/>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>1.068544215975809</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.5750422146295873</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>0.6187132142691636</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>1.033704124000581</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>26.88296017811764</v>
+      </c>
       <c r="I18" s="10" t="inlineStr">
         <is>
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="J18" s="9" t="n"/>
-      <c r="K18" s="9" t="n"/>
-      <c r="L18" s="9" t="n"/>
-      <c r="M18" s="9" t="n"/>
-      <c r="N18" s="9" t="n"/>
-      <c r="O18" s="9" t="n"/>
-      <c r="P18" s="9" t="n"/>
+      <c r="J18" s="9" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K18" s="9" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
+        </is>
+      </c>
+      <c r="L18" s="9" t="n">
+        <v>1.068544215975809</v>
+      </c>
+      <c r="M18" s="9" t="n">
+        <v>0.5750422146295873</v>
+      </c>
+      <c r="N18" s="9" t="n">
+        <v>0.6187132142691636</v>
+      </c>
+      <c r="O18" s="9" t="n">
+        <v>1.033704124000581</v>
+      </c>
+      <c r="P18" s="9" t="n">
+        <v>26.88296017811764</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
@@ -5963,13 +6395,31 @@
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="B10" s="5" t="n"/>
-      <c r="C10" s="5" t="n"/>
-      <c r="D10" s="5" t="n"/>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="5" t="n"/>
-      <c r="G10" s="5" t="n"/>
-      <c r="H10" s="5" t="n"/>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>{'weights': 'distance', 'n_neighbors': 3}</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>0.06233812930092306</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.1632443739181603</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>1.666871086652308</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0.2496760487129734</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>33.73773009935556</v>
+      </c>
       <c r="I10" s="10" t="inlineStr">
         <is>
           <t>K-Neighbors Regressor</t>
@@ -6245,13 +6695,31 @@
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="B18" s="5" t="n"/>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 60, 'max_samples': 1.0, 'max_features': 0.6}</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>0.06552915347075119</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.1821546543887726</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>2.382204980059924</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>0.255986627523297</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>36.37816404012864</v>
+      </c>
       <c r="I18" s="10" t="inlineStr">
         <is>
           <t>BaggingRegressor</t>
@@ -6751,13 +7219,31 @@
           <t>K-Neighbors Regressor</t>
         </is>
       </c>
-      <c r="B10" s="5" t="n"/>
-      <c r="C10" s="5" t="n"/>
-      <c r="D10" s="5" t="n"/>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="5" t="n"/>
-      <c r="G10" s="5" t="n"/>
-      <c r="H10" s="5" t="n"/>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>{'weights': 'uniform', 'n_neighbors': 9}</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>0.805483277707234</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.6113213625379752</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0.469426522995507</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0.8974872019740638</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>32.09916531288695</v>
+      </c>
       <c r="I10" s="10" t="inlineStr">
         <is>
           <t>K-Neighbors Regressor</t>
@@ -7033,13 +7519,31 @@
           <t>BaggingRegressor</t>
         </is>
       </c>
-      <c r="B18" s="5" t="n"/>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>0.8891844026843607</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.7225523156575108</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>0.4984180519552223</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>0.9429657484152649</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>35.4726861658299</v>
+      </c>
       <c r="I18" s="10" t="inlineStr">
         <is>
           <t>BaggingRegressor</t>

</xml_diff>